<commit_message>
Actualización de variable para envio de correo
</commit_message>
<xml_diff>
--- a/Data/Temp/EDS no Incluidas.xlsx
+++ b/Data/Temp/EDS no Incluidas.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10650"/>
   </bookViews>
   <sheets>
-    <sheet name="EDS no incluidas" sheetId="2" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
+    <sheet name="EDS no incluidas Salesforce" sheetId="3" r:id="rId1"/>
+    <sheet name="EDS no incluidas" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="57">
   <si>
     <t>CodigoUnico</t>
   </si>
@@ -76,6 +77,126 @@
   </si>
   <si>
     <t>976</t>
+  </si>
+  <si>
+    <t>No. Recibo sin PCC</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Validación</t>
+  </si>
+  <si>
+    <t>Venta: Nombre PDV</t>
+  </si>
+  <si>
+    <t>Venta: Código Unico PDV</t>
+  </si>
+  <si>
+    <t>Venta: Numero Venta</t>
+  </si>
+  <si>
+    <t>Medio de Pago</t>
+  </si>
+  <si>
+    <t>Código Voucher</t>
+  </si>
+  <si>
+    <t>Venta: Fecha de Transacción</t>
+  </si>
+  <si>
+    <t>Monto</t>
+  </si>
+  <si>
+    <t>Venta: Producto Fidelizable (Gal/m3)</t>
+  </si>
+  <si>
+    <t>Observación</t>
+  </si>
+  <si>
+    <t>50000000210344998EDS3234</t>
+  </si>
+  <si>
+    <t>No Existe en Satelite</t>
+  </si>
+  <si>
+    <t>EDS TERPEL JAVERIANA</t>
+  </si>
+  <si>
+    <t>EDS3234</t>
+  </si>
+  <si>
+    <t>V-0133138756</t>
+  </si>
+  <si>
+    <t>Bono Fidelización</t>
+  </si>
+  <si>
+    <t>Existe en SalesForce</t>
+  </si>
+  <si>
+    <t>EDS2222</t>
+  </si>
+  <si>
+    <t>EDS2223</t>
+  </si>
+  <si>
+    <t>134045454447815243322EDS3226</t>
+  </si>
+  <si>
+    <t>EDS TERPEL AV 68.</t>
+  </si>
+  <si>
+    <t>EDS2224</t>
+  </si>
+  <si>
+    <t>V-0133138944</t>
+  </si>
+  <si>
+    <t>28/03/2022 10:40 AM</t>
+  </si>
+  <si>
+    <t>20006335700EDS3226</t>
+  </si>
+  <si>
+    <t>EDS2225</t>
+  </si>
+  <si>
+    <t>V-0133139128</t>
+  </si>
+  <si>
+    <t>EDS2226</t>
+  </si>
+  <si>
+    <t>20006335701EDS3226</t>
+  </si>
+  <si>
+    <t>EDS2227</t>
+  </si>
+  <si>
+    <t>V-0133139132</t>
+  </si>
+  <si>
+    <t>20006335702EDS3226</t>
+  </si>
+  <si>
+    <t>EDS2228</t>
+  </si>
+  <si>
+    <t>V-0133139138</t>
+  </si>
+  <si>
+    <t>5215EDS3225</t>
+  </si>
+  <si>
+    <t>EDS2229</t>
+  </si>
+  <si>
+    <t>EDS2230</t>
+  </si>
+  <si>
+    <t>EDS2231</t>
   </si>
 </sst>
 </file>
@@ -118,9 +239,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,9 +524,795 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2">
+        <v>74901</v>
+      </c>
+      <c r="I2" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J2">
+        <v>10000</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3">
+        <v>544416</v>
+      </c>
+      <c r="I3" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J3">
+        <v>10000</v>
+      </c>
+      <c r="L3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4">
+        <v>924915</v>
+      </c>
+      <c r="I4" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J4">
+        <v>10000</v>
+      </c>
+      <c r="L4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5">
+        <v>30402</v>
+      </c>
+      <c r="I5" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J5">
+        <v>10000</v>
+      </c>
+      <c r="L5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6">
+        <v>74901</v>
+      </c>
+      <c r="I6" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J6">
+        <v>10000</v>
+      </c>
+      <c r="L6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7">
+        <v>544416</v>
+      </c>
+      <c r="I7" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J7">
+        <v>10000</v>
+      </c>
+      <c r="L7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8">
+        <v>924915</v>
+      </c>
+      <c r="I8" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J8">
+        <v>10000</v>
+      </c>
+      <c r="L8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9">
+        <v>30402</v>
+      </c>
+      <c r="I9" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J9">
+        <v>10000</v>
+      </c>
+      <c r="L9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>1.34045E+20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10">
+        <v>743316</v>
+      </c>
+      <c r="I10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10">
+        <v>5000</v>
+      </c>
+      <c r="L10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>20006335700</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11">
+        <v>684619</v>
+      </c>
+      <c r="I11" s="3">
+        <v>44716.595833333333</v>
+      </c>
+      <c r="J11">
+        <v>10000</v>
+      </c>
+      <c r="L11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>20006335700</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12">
+        <v>371514</v>
+      </c>
+      <c r="I12" s="3">
+        <v>44716.595833333333</v>
+      </c>
+      <c r="J12">
+        <v>10000</v>
+      </c>
+      <c r="L12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>20006335701</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13">
+        <v>763613</v>
+      </c>
+      <c r="I13" s="3">
+        <v>44716.595833333333</v>
+      </c>
+      <c r="J13">
+        <v>10000</v>
+      </c>
+      <c r="L13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>20006335702</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14">
+        <v>151011</v>
+      </c>
+      <c r="I14" s="3">
+        <v>44716.595833333333</v>
+      </c>
+      <c r="J14">
+        <v>10000</v>
+      </c>
+      <c r="L14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15">
+        <v>74901</v>
+      </c>
+      <c r="I15" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J15">
+        <v>10000</v>
+      </c>
+      <c r="L15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16">
+        <v>544416</v>
+      </c>
+      <c r="I16" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J16">
+        <v>10000</v>
+      </c>
+      <c r="L16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17">
+        <v>924915</v>
+      </c>
+      <c r="I17" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J17">
+        <v>10000</v>
+      </c>
+      <c r="L17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18">
+        <v>30402</v>
+      </c>
+      <c r="I18" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J18">
+        <v>10000</v>
+      </c>
+      <c r="L18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19">
+        <v>74901</v>
+      </c>
+      <c r="I19" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J19">
+        <v>10000</v>
+      </c>
+      <c r="L19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20">
+        <v>544416</v>
+      </c>
+      <c r="I20" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J20">
+        <v>10000</v>
+      </c>
+      <c r="L20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21">
+        <v>924915</v>
+      </c>
+      <c r="I21" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J21">
+        <v>10000</v>
+      </c>
+      <c r="L21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>5E+16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22">
+        <v>30402</v>
+      </c>
+      <c r="I22" s="3">
+        <v>44776.442361111112</v>
+      </c>
+      <c r="J22">
+        <v>10000</v>
+      </c>
+      <c r="L22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
@@ -489,7 +1398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>